<commit_message>
Adjust indentation and alignment
</commit_message>
<xml_diff>
--- a/docs_cn/dictionary_tree.xlsx
+++ b/docs_cn/dictionary_tree.xlsx
@@ -66,10 +66,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> &gt;&gt;&gt;  GBDT, random forest etc. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve"> &gt;&gt;&gt; HMM, Naive Bayes etc. </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -91,6 +87,10 @@
   </si>
   <si>
     <t xml:space="preserve"> &gt;&gt;&gt; KNN </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &gt;&gt;&gt; GBDT, random forest etc. </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -190,8 +190,36 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
 </styleSheet>
 </file>
 
@@ -483,7 +511,7 @@
   <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -546,7 +574,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -557,7 +585,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -568,7 +596,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -579,7 +607,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -590,7 +618,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -601,7 +629,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -611,7 +639,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>

</xml_diff>

<commit_message>
split utis.py into serveral files.
</commit_message>
<xml_diff>
--- a/docs_cn/dictionary_tree.xlsx
+++ b/docs_cn/dictionary_tree.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>docs_cn</t>
   </si>
@@ -62,18 +62,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> &gt;&gt;&gt; Clustering algorithms. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> &gt;&gt;&gt; HMM, Naive Bayes etc. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> &gt;&gt;&gt; Decision tree, regression tree etc. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve"> &gt;&gt;&gt; Pictures used in examples. </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -82,18 +70,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> &gt;&gt;&gt; Linear regression, logistic regression etc. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> &gt;&gt;&gt; KNN </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> &gt;&gt;&gt; GBDT, random forest etc. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>daft</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -106,7 +82,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> &gt;&gt;&gt; Collaborative filtering, FP-growth etc. </t>
+    <t>utils</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &gt;&gt;&gt; Utils functions and classes.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &gt;&gt;&gt; ALS. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &gt;&gt;&gt; HMM and Gaussian Naive Bayes.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &gt;&gt;&gt; GBDT, Random Forest and Isolation Forest.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &gt;&gt;&gt; Linear Regression, Logistic Regression and Ridge. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &gt;&gt;&gt; Decision Tree, Regression Tree and Isolation Tree.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &gt;&gt;&gt; KNN. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &gt;&gt;&gt; K-Means.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -524,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F14"/>
+  <dimension ref="B1:F15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -579,7 +587,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -590,7 +598,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -598,10 +606,10 @@
       <c r="B7" s="3"/>
       <c r="C7" s="1"/>
       <c r="D7" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -612,7 +620,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -623,7 +631,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -634,7 +642,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -645,7 +653,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -653,10 +661,10 @@
       <c r="B12" s="3"/>
       <c r="C12" s="1"/>
       <c r="D12" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -667,20 +675,31 @@
         <v>7</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="2:6" ht="15.75">
-      <c r="B14" s="1"/>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="2:6" ht="15.75">
+      <c r="B15" s="1"/>
+      <c r="C15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>